<commit_message>
Excel Database and Awsome fonts Added
</commit_message>
<xml_diff>
--- a/DatabaseCitys.xlsx
+++ b/DatabaseCitys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CAMMM-Web-Tool-1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CAMMM-Web-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77AA4B56-AF2D-4531-8709-D90367483F74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84968975-5A18-474F-AD4B-1B42C988EF12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29310" yWindow="5760" windowWidth="17865" windowHeight="15435" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -535,366 +535,366 @@
   <dimension ref="A1:Q7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="59.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="61" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="59.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="61" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1"/>
-      <c r="Q1" s="1" t="s">
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="2" t="s">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="1"/>
+      <c r="Q2" s="2"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>3</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>65666</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>123</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>50</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>19</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>431.5</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>1.78</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>4115</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="L3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="M3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="N3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="O3" s="2">
+      <c r="O3" s="1">
         <v>-73.709999999999994</v>
       </c>
-      <c r="P3" s="2">
+      <c r="P3" s="1">
         <v>45.53</v>
       </c>
-      <c r="Q3" s="2">
+      <c r="Q3" s="1">
         <v>10.45</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>6</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>78888</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>456</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>35</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>20</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>414.6</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>1.8</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>4341</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="L4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="M4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="N4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="O4" s="2">
+      <c r="O4" s="1">
         <v>16.39</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="Q4" s="1">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>6</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>44444</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>36</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>135</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>101.9</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>5.5750000000000002</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>54710</v>
       </c>
-      <c r="K5" s="2" t="s">
+      <c r="K5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="L5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="M5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="N5" s="2" t="s">
+      <c r="N5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="O5" s="2">
+      <c r="O5" s="1">
         <v>2.13</v>
       </c>
-      <c r="P5" s="2">
+      <c r="P5" s="1">
         <v>41.38</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="Q5" s="1">
         <v>11.81</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>2</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>3333333</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>66</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>222</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>15</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>525.20000000000005</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>1.75</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>3388</v>
       </c>
-      <c r="K6" s="2" t="s">
+      <c r="K6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="L6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="M6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="O6" s="2">
+      <c r="O6" s="1">
         <v>19.12</v>
       </c>
-      <c r="P6" s="2">
+      <c r="P6" s="1">
         <v>47.48</v>
       </c>
-      <c r="Q6" s="2">
+      <c r="Q6" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>4</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>777777</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>77</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>222</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>10</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>234.5</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="1">
         <v>1648</v>
       </c>
-      <c r="K7" s="2" t="s">
+      <c r="K7" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="L7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="M7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N7" s="2" t="s">
+      <c r="N7" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="2">
+      <c r="O7" s="1">
         <v>-71.260000000000005</v>
       </c>
-      <c r="P7" s="2">
+      <c r="P7" s="1">
         <v>46.78</v>
       </c>
-      <c r="Q7" s="2">
+      <c r="Q7" s="1">
         <v>11.3</v>
       </c>
     </row>
@@ -918,5 +918,6 @@
     <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixing map ui styling and city metrics excel to json python
Co-authored-by: Omar Ortiz Meraz <omar.ortizmeraz@mail.concordia.ca>
</commit_message>
<xml_diff>
--- a/DatabaseCitys.xlsx
+++ b/DatabaseCitys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CAMMM-Web-Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fn24x\CAMMM-Web-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84968975-5A18-474F-AD4B-1B42C988EF12}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21ECC1B2-86A8-4678-A99B-6C30F479A67E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -210,8 +210,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -534,106 +537,106 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E70725-99F3-4F19-8F96-434E9A453C7B}">
   <dimension ref="A1:Q7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="59.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="59.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="61" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="15" max="15" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2" t="s">
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
       <c r="O2" s="1" t="s">
         <v>15</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="2"/>
+      <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -655,8 +658,8 @@
       <c r="G3" s="1">
         <v>19</v>
       </c>
-      <c r="H3" s="1">
-        <v>431.5</v>
+      <c r="H3" s="2">
+        <v>365.65</v>
       </c>
       <c r="I3" s="1">
         <v>1.78</v>
@@ -686,7 +689,7 @@
         <v>10.45</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -739,7 +742,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -761,8 +764,8 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="H5" s="1">
-        <v>101.9</v>
+      <c r="H5" s="2">
+        <v>101.35</v>
       </c>
       <c r="I5" s="1">
         <v>5.5750000000000002</v>
@@ -792,7 +795,7 @@
         <v>11.81</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>28</v>
       </c>
@@ -845,7 +848,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -867,8 +870,8 @@
       <c r="G7" s="1">
         <v>10</v>
       </c>
-      <c r="H7" s="1">
-        <v>234.5</v>
+      <c r="H7" s="2">
+        <v>453.38</v>
       </c>
       <c r="I7" s="1">
         <v>0.56999999999999995</v>
@@ -918,6 +921,6 @@
     <mergeCell ref="G1:G2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working on XLS to JSON python code
Co-authored-by: Omar Ortiz Meraz <omar.ortizmeraz@mail.concordia.ca>
</commit_message>
<xml_diff>
--- a/DatabaseCitys.xlsx
+++ b/DatabaseCitys.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CAMMM-Web-Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fn24x\CAMMM-Web-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984575AD-15C0-4A60-A753-F9E760CE4B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE5CC47-7187-42A8-8923-4EBC237F71A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -34,17 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="50">
   <si>
     <t>name</t>
   </si>
   <si>
-    <t>NumTransportSystem</t>
-  </si>
-  <si>
-    <t>NumBusStops</t>
-  </si>
-  <si>
     <t>NumRailStations</t>
   </si>
   <si>
@@ -169,6 +163,27 @@
   </si>
   <si>
     <t>Montreal</t>
+  </si>
+  <si>
+    <t>NumTransitSystems</t>
+  </si>
+  <si>
+    <t>NumStops</t>
+  </si>
+  <si>
+    <t>NumLines</t>
+  </si>
+  <si>
+    <t>AvgDisStops</t>
+  </si>
+  <si>
+    <t>Bus</t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>Metro</t>
   </si>
 </sst>
 </file>
@@ -210,7 +225,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -220,6 +235,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -535,125 +556,139 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E70725-99F3-4F19-8F96-434E9A453C7B}">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:O6"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="59.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="61" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.44140625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="K1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="N2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="O2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="P2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>8</v>
-      </c>
+      <c r="Q2" s="4"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="1" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="G3" s="1">
         <v>-73.709999999999994</v>
@@ -670,49 +705,49 @@
       <c r="K3" s="1">
         <v>65666</v>
       </c>
-      <c r="L3" s="1">
+      <c r="N3" s="1">
         <v>123</v>
       </c>
-      <c r="M3" s="1">
+      <c r="O3" s="1">
         <v>50</v>
       </c>
-      <c r="N3" s="1">
+      <c r="P3" s="1">
         <v>19</v>
       </c>
-      <c r="O3" s="2">
+      <c r="Q3" s="2">
         <v>365.65</v>
       </c>
-      <c r="P3" s="1">
+      <c r="R3" s="1">
         <v>1.78</v>
       </c>
-      <c r="Q3" s="1">
+      <c r="S3" s="1">
         <v>4115</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G4" s="1">
         <v>16.39</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I4" s="1">
         <v>11</v>
@@ -723,43 +758,43 @@
       <c r="K4" s="1">
         <v>78888</v>
       </c>
-      <c r="L4" s="1">
+      <c r="N4" s="1">
         <v>456</v>
       </c>
-      <c r="M4" s="1">
+      <c r="O4" s="1">
         <v>35</v>
       </c>
-      <c r="N4" s="1">
+      <c r="P4" s="1">
         <v>20</v>
       </c>
-      <c r="O4" s="1">
+      <c r="Q4" s="1">
         <v>414.6</v>
       </c>
-      <c r="P4" s="1">
+      <c r="R4" s="1">
         <v>1.8</v>
       </c>
-      <c r="Q4" s="1">
+      <c r="S4" s="1">
         <v>4341</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="E5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G5" s="1">
         <v>2.13</v>
@@ -776,43 +811,43 @@
       <c r="K5" s="1">
         <v>44444</v>
       </c>
-      <c r="L5" s="1">
+      <c r="N5" s="1">
         <v>36</v>
       </c>
-      <c r="M5" s="1">
+      <c r="O5" s="1">
         <v>135</v>
       </c>
-      <c r="N5" s="1">
+      <c r="P5" s="1">
         <v>1</v>
       </c>
-      <c r="O5" s="2">
+      <c r="Q5" s="2">
         <v>101.35</v>
       </c>
-      <c r="P5" s="1">
+      <c r="R5" s="1">
         <v>5.5750000000000002</v>
       </c>
-      <c r="Q5" s="1">
+      <c r="S5" s="1">
         <v>54710</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>30</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G6" s="1">
         <v>19.12</v>
@@ -829,43 +864,43 @@
       <c r="K6" s="1">
         <v>3333333</v>
       </c>
-      <c r="L6" s="1">
+      <c r="N6" s="1">
         <v>66</v>
       </c>
-      <c r="M6" s="1">
+      <c r="O6" s="1">
         <v>222</v>
       </c>
-      <c r="N6" s="1">
+      <c r="P6" s="1">
         <v>15</v>
       </c>
-      <c r="O6" s="1">
+      <c r="Q6" s="1">
         <v>525.20000000000005</v>
       </c>
-      <c r="P6" s="1">
+      <c r="R6" s="1">
         <v>1.75</v>
       </c>
-      <c r="Q6" s="1">
+      <c r="S6" s="1">
         <v>3388</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G7" s="1">
         <v>-71.260000000000005</v>
@@ -882,43 +917,40 @@
       <c r="K7" s="1">
         <v>777777</v>
       </c>
-      <c r="L7" s="1">
+      <c r="N7" s="1">
         <v>77</v>
       </c>
-      <c r="M7" s="1">
+      <c r="O7" s="1">
         <v>222</v>
       </c>
-      <c r="N7" s="1">
+      <c r="P7" s="1">
         <v>10</v>
       </c>
-      <c r="O7" s="2">
+      <c r="Q7" s="2">
         <v>453.38</v>
       </c>
-      <c r="P7" s="1">
+      <c r="R7" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="Q7" s="1">
+      <c r="S7" s="1">
         <v>1648</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="13">
+    <mergeCell ref="R1:R2"/>
+    <mergeCell ref="S1:S2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="K1:M1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:A2"/>
-    <mergeCell ref="O1:O2"/>
-    <mergeCell ref="P1:P2"/>
     <mergeCell ref="Q1:Q2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="B1:B2"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="K1:K2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:N2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Re update to excel
</commit_message>
<xml_diff>
--- a/DatabaseCitys.xlsx
+++ b/DatabaseCitys.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CAMMM-Web-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00549BDF-43E9-4B0F-B310-0D38B645EE8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB735453-086F-4E38-A5B1-9DB541F4024A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="18210" windowHeight="10320" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -78,12 +78,6 @@
     <t>Montréal</t>
   </si>
   <si>
-    <t>"montreal_D_CD","montreal_D_CL"</t>
-  </si>
-  <si>
-    <t>"montreal_N_CD","montreal_N_CL"</t>
-  </si>
-  <si>
     <t>Vienna</t>
   </si>
   <si>
@@ -96,33 +90,9 @@
     <t>Quebec</t>
   </si>
   <si>
-    <t>"vienna_D_CD", "vienna_D_CL"</t>
-  </si>
-  <si>
-    <t>"vienna_N_CD","vienna_N_CL"</t>
-  </si>
-  <si>
     <t> 48.20</t>
   </si>
   <si>
-    <t>"barcelona_D_CD","barcelona_D_CL","barcelona_D_EV"</t>
-  </si>
-  <si>
-    <t>"budapest_D_CD","budapest_D_CL"</t>
-  </si>
-  <si>
-    <t>"budapest_N_CD","budapest_N_CL"</t>
-  </si>
-  <si>
-    <t>"quebec_D_CD","quebec_D_CL"</t>
-  </si>
-  <si>
-    <t>"quebec_N_CD","quebec_N_CL"</t>
-  </si>
-  <si>
-    <t>"barcelona_N_CD","barcelona_N_CL","barcelona_N_EV"</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
@@ -184,6 +154,36 @@
   </si>
   <si>
     <t>ckpwzbcwp51pt17njpumzg0hq</t>
+  </si>
+  <si>
+    <t>montreal_D_CD,montreal_D_CL</t>
+  </si>
+  <si>
+    <t>vienna_D_CD,vienna_D_CL</t>
+  </si>
+  <si>
+    <t>barcelona_D_CD,barcelona_D_CL,barcelona_D_EV</t>
+  </si>
+  <si>
+    <t>budapest_D_CD,budapest_D_CL</t>
+  </si>
+  <si>
+    <t>quebec_D_CD,quebec_D_CL</t>
+  </si>
+  <si>
+    <t>montreal_N_CD,montreal_N_CL</t>
+  </si>
+  <si>
+    <t>vienna_N_CD,vienna_N_CL</t>
+  </si>
+  <si>
+    <t>barcelona_N_CD,barcelona_N_CL,barcelona_N_EV</t>
+  </si>
+  <si>
+    <t>budapest_N_CD,budapest_N_CL</t>
+  </si>
+  <si>
+    <t>quebec_N_CD,quebec_N_CL</t>
   </si>
 </sst>
 </file>
@@ -558,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E70725-99F3-4F19-8F96-434E9A453C7B}">
   <dimension ref="A1:AC7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AL4" sqref="AL4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +586,7 @@
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -611,30 +611,30 @@
         <v>10</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
       <c r="N1" s="5" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
       <c r="Q1" s="5" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="U1" s="5"/>
       <c r="V1" s="5"/>
       <c r="W1" s="5" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="X1" s="5"/>
       <c r="Y1" s="5"/>
@@ -665,49 +665,49 @@
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
       <c r="K2" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="Y2" s="3" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="Z2" s="4" t="s">
         <v>1</v>
@@ -718,22 +718,22 @@
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="G3" s="3">
         <v>-73.709999999999994</v>
@@ -807,28 +807,28 @@
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>41</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="G4" s="3">
         <v>16.39</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I4" s="3">
         <v>11</v>
@@ -896,22 +896,22 @@
     </row>
     <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="G5" s="3">
         <v>2.13</v>
@@ -985,22 +985,22 @@
     </row>
     <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="G6" s="3">
         <v>19.12</v>
@@ -1074,22 +1074,22 @@
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="G7" s="3">
         <v>-71.260000000000005</v>
@@ -1163,11 +1163,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="T1:V1"/>
-    <mergeCell ref="W1:Y1"/>
-    <mergeCell ref="AA1:AA2"/>
-    <mergeCell ref="AB1:AB2"/>
-    <mergeCell ref="AC1:AC2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
     <mergeCell ref="N1:P1"/>
@@ -1180,6 +1175,11 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="G1:H1"/>
+    <mergeCell ref="T1:V1"/>
+    <mergeCell ref="W1:Y1"/>
+    <mergeCell ref="AA1:AA2"/>
+    <mergeCell ref="AB1:AB2"/>
+    <mergeCell ref="AC1:AC2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Finishing conversion py for xls to json
</commit_message>
<xml_diff>
--- a/DatabaseCitys.xlsx
+++ b/DatabaseCitys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fn24x\CAMMM-Web-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87179A59-E38C-49D0-83F2-2AFBC697BC67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C148FA-48F7-42F0-AE54-906ADFDDCE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24" yWindow="24" windowWidth="19176" windowHeight="10176" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
   <si>
     <t>City</t>
   </si>
@@ -135,9 +135,6 @@
     <t>ckqtuaktz0c3317mopggbopa1</t>
   </si>
   <si>
-    <t> 48.20</t>
-  </si>
-  <si>
     <t>vienna_N_CD,vienna_N_CL</t>
   </si>
   <si>
@@ -205,6 +202,12 @@
   </si>
   <si>
     <t>quebec-bus_CD, quebec-bus_CL</t>
+  </si>
+  <si>
+    <t>Québec</t>
+  </si>
+  <si>
+    <t>Wien</t>
   </si>
 </sst>
 </file>
@@ -246,13 +249,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -574,7 +583,7 @@
   <dimension ref="A1:AG7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+      <selection activeCell="R3" sqref="R3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -603,85 +612,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3" t="s">
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3" t="s">
+      <c r="S1" s="5"/>
+      <c r="T1" s="5"/>
+      <c r="U1" s="5"/>
+      <c r="V1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
-      <c r="Y1" s="3"/>
-      <c r="Z1" s="3" t="s">
+      <c r="W1" s="5"/>
+      <c r="X1" s="5"/>
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="3"/>
-      <c r="AB1" s="3"/>
-      <c r="AC1" s="3"/>
-      <c r="AE1" s="3" t="s">
+      <c r="AA1" s="5"/>
+      <c r="AB1" s="5"/>
+      <c r="AC1" s="5"/>
+      <c r="AE1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AF1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AG1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
       <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
@@ -745,9 +754,9 @@
       <c r="AD2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
-      <c r="AG2" s="3"/>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5"/>
+      <c r="AG2" s="5"/>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -762,16 +771,16 @@
       <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="1">
+      <c r="E3" s="3">
         <v>-73.709999999999994</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="3">
         <v>45.53</v>
       </c>
-      <c r="G3" s="1">
+      <c r="G3" s="3">
         <v>10.45</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="3">
         <v>2</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -780,64 +789,65 @@
       <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="4">
         <v>11355</v>
       </c>
-      <c r="L3" s="1">
+      <c r="L3" s="4">
         <v>217</v>
       </c>
-      <c r="M3" s="1">
+      <c r="M3" s="4">
         <v>318</v>
       </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
-      <c r="P3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="1">
+      <c r="O3" s="4">
+        <v>0</v>
+      </c>
+      <c r="P3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="4">
         <v>0</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="S3" s="1">
+      <c r="S3" s="4">
         <v>69</v>
       </c>
-      <c r="T3" s="1">
+      <c r="T3" s="4">
         <v>4</v>
       </c>
-      <c r="U3" s="1">
+      <c r="U3" s="4">
         <v>2787</v>
       </c>
-      <c r="W3" s="1">
-        <v>0</v>
-      </c>
-      <c r="X3" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="1">
+      <c r="W3" s="4">
+        <v>0</v>
+      </c>
+      <c r="X3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="4"/>
+      <c r="AA3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="4">
         <v>19</v>
       </c>
-      <c r="AE3" s="1">
+      <c r="AE3" s="3">
         <v>365.65</v>
       </c>
-      <c r="AF3" s="1">
+      <c r="AF3" s="3">
         <v>1.78</v>
       </c>
-      <c r="AG3" s="1">
+      <c r="AG3" s="4">
         <v>4115</v>
       </c>
     </row>
@@ -846,7 +856,7 @@
         <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>31</v>
@@ -854,375 +864,375 @@
       <c r="D4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="3">
         <v>16.39</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3">
+        <v>48.2</v>
+      </c>
+      <c r="G4" s="3">
+        <v>11</v>
+      </c>
+      <c r="H4" s="3">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G4" s="1">
-        <v>11</v>
-      </c>
-      <c r="H4" s="1">
-        <v>3</v>
-      </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="4">
+        <v>9653</v>
+      </c>
+      <c r="L4" s="4">
+        <v>451</v>
+      </c>
+      <c r="M4" s="4">
+        <v>331</v>
+      </c>
+      <c r="O4" s="4">
+        <v>0</v>
+      </c>
+      <c r="P4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>0</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K4" s="1">
-        <v>9653</v>
-      </c>
-      <c r="L4" s="1">
-        <v>451</v>
-      </c>
-      <c r="M4" s="1">
-        <v>331</v>
-      </c>
-      <c r="O4" s="1">
-        <v>0</v>
-      </c>
-      <c r="P4" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="1">
-        <v>0</v>
-      </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="4">
+        <v>768</v>
+      </c>
+      <c r="T4" s="4">
+        <v>37</v>
+      </c>
+      <c r="U4" s="4">
+        <v>655</v>
+      </c>
+      <c r="V4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S4" s="1">
-        <v>768</v>
-      </c>
-      <c r="T4" s="1">
-        <v>37</v>
-      </c>
-      <c r="U4" s="1">
-        <v>655</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="W4" s="1">
+      <c r="W4" s="4">
         <v>3360</v>
       </c>
-      <c r="X4" s="1">
+      <c r="X4" s="4">
         <v>135</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="Y4" s="4">
         <v>346</v>
       </c>
-      <c r="AA4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC4" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD4" s="1">
+      <c r="Z4" s="4"/>
+      <c r="AA4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="4">
         <v>20</v>
       </c>
-      <c r="AE4" s="1">
+      <c r="AE4" s="3">
         <v>414.6</v>
       </c>
-      <c r="AF4" s="1">
+      <c r="AF4" s="3">
         <v>1.8</v>
       </c>
-      <c r="AG4" s="1">
+      <c r="AG4" s="4">
         <v>4341</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="3">
+        <v>2.13</v>
+      </c>
+      <c r="F5" s="3">
+        <v>41.38</v>
+      </c>
+      <c r="G5" s="3">
+        <v>11.81</v>
+      </c>
+      <c r="H5" s="3">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E5" s="1">
-        <v>2.13</v>
-      </c>
-      <c r="F5" s="1">
-        <v>41.38</v>
-      </c>
-      <c r="G5" s="1">
-        <v>11.81</v>
-      </c>
-      <c r="H5" s="1">
-        <v>2</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J5" s="1" t="s">
+      <c r="K5" s="4">
+        <v>4067</v>
+      </c>
+      <c r="L5" s="4">
+        <v>277</v>
+      </c>
+      <c r="M5" s="4">
+        <v>277</v>
+      </c>
+      <c r="O5" s="4">
+        <v>0</v>
+      </c>
+      <c r="P5" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="4">
+        <v>0</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="K5" s="1">
-        <v>4067</v>
-      </c>
-      <c r="L5" s="1">
-        <v>277</v>
-      </c>
-      <c r="M5" s="1">
-        <v>277</v>
-      </c>
-      <c r="O5" s="1">
-        <v>0</v>
-      </c>
-      <c r="P5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="1">
-        <v>0</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S5" s="1">
+      <c r="S5" s="4">
         <v>155</v>
       </c>
-      <c r="T5" s="1">
+      <c r="T5" s="4">
         <v>10</v>
       </c>
-      <c r="U5" s="1">
+      <c r="U5" s="4">
         <v>2669</v>
       </c>
-      <c r="W5" s="1">
-        <v>0</v>
-      </c>
-      <c r="X5" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="1">
+      <c r="W5" s="4">
+        <v>0</v>
+      </c>
+      <c r="X5" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="4"/>
+      <c r="AA5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="4">
         <v>15</v>
       </c>
-      <c r="AE5" s="1">
+      <c r="AE5" s="3">
         <v>101.35</v>
       </c>
-      <c r="AF5" s="1">
+      <c r="AF5" s="3">
         <v>1.66</v>
       </c>
-      <c r="AG5" s="1">
+      <c r="AG5" s="4">
         <v>16420</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="3">
+        <v>19.12</v>
+      </c>
+      <c r="F6" s="3">
+        <v>47.48</v>
+      </c>
+      <c r="G6" s="3">
+        <v>10</v>
+      </c>
+      <c r="H6" s="3">
+        <v>4</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="1">
-        <v>19.12</v>
-      </c>
-      <c r="F6" s="1">
-        <v>47.48</v>
-      </c>
-      <c r="G6" s="1">
-        <v>10</v>
-      </c>
-      <c r="H6" s="1">
-        <v>4</v>
-      </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="4">
+        <v>10745</v>
+      </c>
+      <c r="L6" s="4">
+        <v>298</v>
+      </c>
+      <c r="M6" s="4">
+        <v>449</v>
+      </c>
+      <c r="N6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="K6" s="1">
-        <v>10745</v>
-      </c>
-      <c r="L6" s="1">
-        <v>298</v>
-      </c>
-      <c r="M6" s="1">
-        <v>449</v>
-      </c>
-      <c r="N6" s="1" t="s">
+      <c r="O6" s="4">
+        <v>170</v>
+      </c>
+      <c r="P6" s="4">
+        <v>109</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>1056</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="O6" s="1">
-        <v>170</v>
-      </c>
-      <c r="P6" s="1">
-        <v>109</v>
-      </c>
-      <c r="Q6" s="1">
-        <v>1056</v>
-      </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="4">
+        <v>73</v>
+      </c>
+      <c r="T6" s="4">
+        <v>5</v>
+      </c>
+      <c r="U6" s="4">
+        <v>1121</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="S6" s="1">
-        <v>73</v>
-      </c>
-      <c r="T6" s="1">
-        <v>5</v>
-      </c>
-      <c r="U6" s="1">
-        <v>1121</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="W6" s="1">
+      <c r="W6" s="4">
         <v>851</v>
       </c>
-      <c r="X6" s="1">
+      <c r="X6" s="4">
         <v>37</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="Y6" s="4">
         <v>417</v>
       </c>
-      <c r="AA6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="1">
+      <c r="Z6" s="4"/>
+      <c r="AA6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="4">
         <v>33</v>
       </c>
-      <c r="AE6" s="1">
+      <c r="AE6" s="3">
         <v>525.20000000000005</v>
       </c>
-      <c r="AF6" s="1">
+      <c r="AF6" s="3">
         <v>1.75</v>
       </c>
-      <c r="AG6" s="1">
+      <c r="AG6" s="4">
         <v>3388</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="3">
+        <v>-71.260000000000005</v>
+      </c>
+      <c r="F7" s="3">
+        <v>46.78</v>
+      </c>
+      <c r="G7" s="3">
+        <v>11.3</v>
+      </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="1">
-        <v>-71.260000000000005</v>
-      </c>
-      <c r="F7" s="1">
-        <v>46.78</v>
-      </c>
-      <c r="G7" s="1">
-        <v>11.3</v>
-      </c>
-      <c r="H7" s="1">
-        <v>1</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J7" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="K7" s="1">
+      <c r="K7" s="4">
         <v>17368</v>
       </c>
-      <c r="L7" s="1">
+      <c r="L7" s="4">
         <v>318</v>
       </c>
-      <c r="M7" s="1">
+      <c r="M7" s="4">
         <v>338</v>
       </c>
-      <c r="O7" s="1">
-        <v>0</v>
-      </c>
-      <c r="P7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="1">
-        <v>0</v>
-      </c>
-      <c r="S7" s="1">
-        <v>0</v>
-      </c>
-      <c r="T7" s="1">
-        <v>0</v>
-      </c>
-      <c r="U7" s="1">
-        <v>0</v>
-      </c>
-      <c r="W7" s="1">
-        <v>0</v>
-      </c>
-      <c r="X7" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="1">
+      <c r="O7" s="4">
+        <v>0</v>
+      </c>
+      <c r="P7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="4">
+        <v>0</v>
+      </c>
+      <c r="S7" s="4">
+        <v>0</v>
+      </c>
+      <c r="T7" s="4">
+        <v>0</v>
+      </c>
+      <c r="U7" s="4">
+        <v>0</v>
+      </c>
+      <c r="W7" s="4">
+        <v>0</v>
+      </c>
+      <c r="X7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="4"/>
+      <c r="AA7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="4">
         <v>6</v>
       </c>
-      <c r="AE7" s="1">
+      <c r="AE7" s="3">
         <v>453.38</v>
       </c>
-      <c r="AF7" s="1">
+      <c r="AF7" s="3">
         <v>0.53</v>
       </c>
-      <c r="AG7" s="1">
+      <c r="AG7" s="4">
         <v>1173</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -1231,8 +1241,12 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="Z1:AC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
@@ -1240,6 +1254,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BFE9A4688917F64EA5EF44A4A73B6A0B" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1d0e5df5db596ad1f7ae9b1118af9b3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5b1997fb-8114-417a-a20b-796df5612ac9" xmlns:ns4="eefc82e4-fec2-46ce-83e1-5271053f7c9b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bb3db480e9256d19dbc0add7ebf3b44" ns3:_="" ns4:_="">
     <xsd:import namespace="5b1997fb-8114-417a-a20b-796df5612ac9"/>
@@ -1456,15 +1479,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1472,6 +1486,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19232968-D0AD-4578-90F9-FB7793DCA679}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24CD1E4A-6B0F-4C5B-8CAD-007A87F29157}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1486,14 +1508,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19232968-D0AD-4578-90F9-FB7793DCA679}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Integrating JSON to UI and adding more city metrics fields
Co-authored-by: Omar Ortiz Meraz <omar.ortizmeraz@mail.concordia.ca>
</commit_message>
<xml_diff>
--- a/DatabaseCitys.xlsx
+++ b/DatabaseCitys.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fn24x\CAMMM-Web-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10C148FA-48F7-42F0-AE54-906ADFDDCE7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E48F54D-8FA4-4C43-A2D2-4741E9F2F86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
   <si>
     <t>City</t>
   </si>
@@ -192,9 +192,6 @@
     <t>Quebec</t>
   </si>
   <si>
-    <t>ckqr0ljp50tnz17k8s2tm4rsh</t>
-  </si>
-  <si>
     <t>ckpwzbcwp51pt17njpumzg0hq</t>
   </si>
   <si>
@@ -208,6 +205,33 @@
   </si>
   <si>
     <t>Wien</t>
+  </si>
+  <si>
+    <t>ckv8617pd0n9g14rxpi45ts4u</t>
+  </si>
+  <si>
+    <t>YearOfStats</t>
+  </si>
+  <si>
+    <t>SourceGTFS</t>
+  </si>
+  <si>
+    <t>https://www.stm.info/en/about/developers</t>
+  </si>
+  <si>
+    <t>DateUpdatedGTFS</t>
+  </si>
+  <si>
+    <t>https://developer.tmb.cat/data</t>
+  </si>
+  <si>
+    <t>https://www.data.gv.at/katalog/dataset/wiener-linien-fahrplandaten-gtfs-wien</t>
+  </si>
+  <si>
+    <t>https://data.europa.eu/it/news/centre-budapest-transport-and-open-mobility-data</t>
+  </si>
+  <si>
+    <t>https://www.rtcquebec.ca/donnees-ouvertes</t>
   </si>
 </sst>
 </file>
@@ -249,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -261,6 +285,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -580,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E70725-99F3-4F19-8F96-434E9A453C7B}">
-  <dimension ref="A1:AG7"/>
+  <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="R3" sqref="R3"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AH10" sqref="AH10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,89 +635,106 @@
     <col min="20" max="20" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="19.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="40.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.109375" style="1"/>
+    <col min="23" max="29" width="9.109375" style="1"/>
+    <col min="30" max="30" width="12.6640625" style="1" customWidth="1"/>
+    <col min="31" max="31" width="9.109375" style="1"/>
+    <col min="32" max="32" width="13.44140625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5546875" style="1" customWidth="1"/>
+    <col min="34" max="34" width="12.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="70.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
+    <row r="1" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5" t="s">
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5" t="s">
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5" t="s">
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="5" t="s">
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="5"/>
-      <c r="X1" s="5"/>
-      <c r="Y1" s="5"/>
-      <c r="Z1" s="5" t="s">
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="5"/>
-      <c r="AB1" s="5"/>
-      <c r="AC1" s="5"/>
-      <c r="AE1" s="5" t="s">
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AE1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="5" t="s">
+      <c r="AF1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="5" t="s">
+      <c r="AG1" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="AH1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AI1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="AJ1" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
+    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
       <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
@@ -754,11 +798,14 @@
       <c r="AD2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6"/>
+      <c r="AJ2" s="6"/>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -850,13 +897,22 @@
       <c r="AG3" s="4">
         <v>4115</v>
       </c>
+      <c r="AH3" s="1">
+        <v>2016</v>
+      </c>
+      <c r="AI3" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="AJ3" s="1">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>31</v>
@@ -946,8 +1002,17 @@
       <c r="AG4" s="4">
         <v>4341</v>
       </c>
+      <c r="AH4" s="1">
+        <v>2019</v>
+      </c>
+      <c r="AI4" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AJ4" s="5">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1039,8 +1104,17 @@
       <c r="AG5" s="4">
         <v>16420</v>
       </c>
+      <c r="AH5" s="1">
+        <v>2015</v>
+      </c>
+      <c r="AI5" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ5" s="5">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
@@ -1138,19 +1212,28 @@
       <c r="AG6" s="4">
         <v>3388</v>
       </c>
+      <c r="AH6" s="1">
+        <v>2014</v>
+      </c>
+      <c r="AI6" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="AJ6" s="5">
+        <v>2021</v>
+      </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>53</v>
       </c>
       <c r="E7" s="3">
         <v>-71.260000000000005</v>
@@ -1165,10 +1248,10 @@
         <v>1</v>
       </c>
       <c r="I7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J7" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="K7" s="4">
         <v>17368</v>
@@ -1228,9 +1311,21 @@
       <c r="AG7" s="4">
         <v>1173</v>
       </c>
+      <c r="AH7" s="1">
+        <v>2016</v>
+      </c>
+      <c r="AI7" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ7" s="5">
+        <v>2021</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="19">
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="I1:I2"/>

</xml_diff>

<commit_message>
Added grid analysis to database XLS
</commit_message>
<xml_diff>
--- a/DatabaseCitys.xlsx
+++ b/DatabaseCitys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fn24x\CAMMM-Web-Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CAMMM-Web-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E48F54D-8FA4-4C43-A2D2-4741E9F2F86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBFADCC-9390-447F-8A64-EB83F2C6ED69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
   <si>
     <t>City</t>
   </si>
@@ -232,13 +232,49 @@
   </si>
   <si>
     <t>https://www.rtcquebec.ca/donnees-ouvertes</t>
+  </si>
+  <si>
+    <t>GridLayers</t>
+  </si>
+  <si>
+    <t>GridStyleURL</t>
+  </si>
+  <si>
+    <t>cl1qihonq002415ng3q7njruw</t>
+  </si>
+  <si>
+    <t>montreal_grid</t>
+  </si>
+  <si>
+    <t>vienna_grid</t>
+  </si>
+  <si>
+    <t>cl1qj5iio000h14lsrpfbbbs7</t>
+  </si>
+  <si>
+    <t>cl1qjcbr9000e15s7ids0qcrt</t>
+  </si>
+  <si>
+    <t>barcelona_grid</t>
+  </si>
+  <si>
+    <t>cl1qjqiij002h14s6sigeccvb</t>
+  </si>
+  <si>
+    <t>budapest_grid</t>
+  </si>
+  <si>
+    <t>cl1qjjphy000g15s7jf1t62sy</t>
+  </si>
+  <si>
+    <t>quebec_grid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +284,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -270,10 +314,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -293,8 +338,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -607,134 +659,146 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E70725-99F3-4F19-8F96-434E9A453C7B}">
-  <dimension ref="A1:AJ7"/>
+  <dimension ref="A1:AL10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AH10" sqref="AH10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2595" topLeftCell="AJ1" activePane="topRight"/>
+      <selection pane="topRight" activeCell="AO6" sqref="AO6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.44140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="32.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="40.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="29" width="9.109375" style="1"/>
-    <col min="30" max="30" width="12.6640625" style="1" customWidth="1"/>
-    <col min="31" max="31" width="9.109375" style="1"/>
-    <col min="32" max="32" width="13.44140625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="12.5546875" style="1" customWidth="1"/>
-    <col min="34" max="34" width="12.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="70.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="16" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="32.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="40.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="9.140625" style="1"/>
+    <col min="27" max="27" width="13.42578125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" style="1" customWidth="1"/>
+    <col min="30" max="30" width="15" style="1" customWidth="1"/>
+    <col min="31" max="31" width="9.140625" style="1"/>
+    <col min="32" max="32" width="13.42578125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5703125" style="1" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="70.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.28515625" style="1" customWidth="1"/>
+    <col min="37" max="37" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="30.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="39" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="1:38" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="I1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6" t="s">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6" t="s">
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6" t="s">
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="6"/>
-      <c r="X1" s="6"/>
-      <c r="Y1" s="6"/>
-      <c r="Z1" s="6" t="s">
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="6"/>
-      <c r="AB1" s="6"/>
-      <c r="AC1" s="6"/>
-      <c r="AE1" s="6" t="s">
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AE1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="6" t="s">
+      <c r="AF1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="6" t="s">
+      <c r="AG1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="6" t="s">
+      <c r="AH1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AI1" s="6" t="s">
+      <c r="AI1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="AJ1" s="6" t="s">
+      <c r="AJ1" s="7" t="s">
         <v>61</v>
       </c>
+      <c r="AK1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL1" s="7" t="s">
+        <v>67</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
       <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
@@ -798,14 +862,16 @@
       <c r="AD2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="6"/>
-      <c r="AF2" s="6"/>
-      <c r="AG2" s="6"/>
-      <c r="AH2" s="6"/>
-      <c r="AI2" s="6"/>
-      <c r="AJ2" s="6"/>
+      <c r="AE2" s="7"/>
+      <c r="AF2" s="7"/>
+      <c r="AG2" s="7"/>
+      <c r="AH2" s="7"/>
+      <c r="AI2" s="7"/>
+      <c r="AJ2" s="7"/>
+      <c r="AK2" s="7"/>
+      <c r="AL2" s="7"/>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -906,8 +972,14 @@
       <c r="AJ3" s="1">
         <v>2021</v>
       </c>
+      <c r="AK3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="AL3" s="6" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1011,8 +1083,14 @@
       <c r="AJ4" s="5">
         <v>2021</v>
       </c>
+      <c r="AK4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL4" s="6" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1113,8 +1191,14 @@
       <c r="AJ5" s="5">
         <v>2021</v>
       </c>
+      <c r="AK5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="AL5" s="6" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
@@ -1221,8 +1305,14 @@
       <c r="AJ6" s="5">
         <v>2021</v>
       </c>
+      <c r="AK6" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="AL6" s="6" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -1320,14 +1410,20 @@
       <c r="AJ7" s="5">
         <v>2021</v>
       </c>
+      <c r="AK7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL7" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AL10" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
+  <mergeCells count="21">
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AL1:AL2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -1336,6 +1432,11 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:F1"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
     <mergeCell ref="AE1:AE2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="AG1:AG2"/>
@@ -1349,15 +1450,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BFE9A4688917F64EA5EF44A4A73B6A0B" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1d0e5df5db596ad1f7ae9b1118af9b3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5b1997fb-8114-417a-a20b-796df5612ac9" xmlns:ns4="eefc82e4-fec2-46ce-83e1-5271053f7c9b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bb3db480e9256d19dbc0add7ebf3b44" ns3:_="" ns4:_="">
     <xsd:import namespace="5b1997fb-8114-417a-a20b-796df5612ac9"/>
@@ -1574,6 +1666,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1581,14 +1682,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19232968-D0AD-4578-90F9-FB7793DCA679}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24CD1E4A-6B0F-4C5B-8CAD-007A87F29157}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1603,6 +1696,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19232968-D0AD-4578-90F9-FB7793DCA679}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Refactoring dropdown and fixing grid analysis layer display
</commit_message>
<xml_diff>
--- a/DatabaseCitys.xlsx
+++ b/DatabaseCitys.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\CAMMM-Web-Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fn24x\CAMMM-Web-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EBFADCC-9390-447F-8A64-EB83F2C6ED69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB8E6F3-1F43-439B-BEF7-711B7724D603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
+    <workbookView xWindow="9210" yWindow="-4570" windowWidth="14850" windowHeight="9180" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
   <si>
     <t>City</t>
   </si>
@@ -268,6 +268,21 @@
   </si>
   <si>
     <t>quebec_grid</t>
+  </si>
+  <si>
+    <t>Flag</t>
+  </si>
+  <si>
+    <t>flags/canada-flag-xs.png</t>
+  </si>
+  <si>
+    <t>flags/austria-flag-xs.png</t>
+  </si>
+  <si>
+    <t>flags/spain-flag-xs.png</t>
+  </si>
+  <si>
+    <t>flags/hungary-flag-xs.png</t>
   </si>
 </sst>
 </file>
@@ -338,10 +353,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -659,146 +674,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E70725-99F3-4F19-8F96-434E9A453C7B}">
-  <dimension ref="A1:AL10"/>
+  <dimension ref="A1:AM10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2595" topLeftCell="AJ1" activePane="topRight"/>
-      <selection pane="topRight" activeCell="AO6" sqref="AO6"/>
+      <pane xSplit="2610" topLeftCell="AJ1" activePane="topRight"/>
+      <selection pane="topRight" activeCell="AM7" sqref="AM7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="40.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="26" width="9.140625" style="1"/>
-    <col min="27" max="27" width="13.42578125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="11.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.44140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="32.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="40.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="9.109375" style="1"/>
+    <col min="27" max="27" width="13.44140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11.88671875" style="1" customWidth="1"/>
     <col min="30" max="30" width="15" style="1" customWidth="1"/>
-    <col min="31" max="31" width="9.140625" style="1"/>
-    <col min="32" max="32" width="13.42578125" style="1" customWidth="1"/>
-    <col min="33" max="33" width="12.5703125" style="1" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="70.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.28515625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="30.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="39" max="16384" width="9.140625" style="1"/>
+    <col min="31" max="31" width="9.109375" style="1"/>
+    <col min="32" max="32" width="13.44140625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5546875" style="1" customWidth="1"/>
+    <col min="34" max="34" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="70.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.33203125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="30.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7" t="s">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7" t="s">
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7" t="s">
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7" t="s">
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
-      <c r="AE1" s="7" t="s">
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AE1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="7" t="s">
+      <c r="AF1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="7" t="s">
+      <c r="AG1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="7" t="s">
+      <c r="AH1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AI1" s="7" t="s">
+      <c r="AI1" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="AJ1" s="7" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="AK1" s="7" t="s">
+      <c r="AK1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AL1" s="7" t="s">
+      <c r="AL1" s="8" t="s">
         <v>67</v>
       </c>
+      <c r="AM1" s="8" t="s">
+        <v>78</v>
+      </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
       <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
@@ -862,16 +881,17 @@
       <c r="AD2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="7"/>
-      <c r="AF2" s="7"/>
-      <c r="AG2" s="7"/>
-      <c r="AH2" s="7"/>
-      <c r="AI2" s="7"/>
-      <c r="AJ2" s="7"/>
-      <c r="AK2" s="7"/>
-      <c r="AL2" s="7"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -978,8 +998,11 @@
       <c r="AL3" s="6" t="s">
         <v>68</v>
       </c>
+      <c r="AM3" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1089,8 +1112,11 @@
       <c r="AL4" s="6" t="s">
         <v>71</v>
       </c>
+      <c r="AM4" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1197,8 +1223,11 @@
       <c r="AL5" s="6" t="s">
         <v>72</v>
       </c>
+      <c r="AM5" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
@@ -1311,8 +1340,11 @@
       <c r="AL6" s="6" t="s">
         <v>74</v>
       </c>
+      <c r="AM6" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -1416,12 +1448,21 @@
       <c r="AL7" s="6" t="s">
         <v>76</v>
       </c>
+      <c r="AM7" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
-      <c r="AL10" s="8"/>
+    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="AL10" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
+    <mergeCell ref="AM1:AM2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="AK1:AK2"/>
     <mergeCell ref="AL1:AL2"/>
     <mergeCell ref="I1:I2"/>
@@ -1438,11 +1479,6 @@
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
@@ -1450,6 +1486,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BFE9A4688917F64EA5EF44A4A73B6A0B" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1d0e5df5db596ad1f7ae9b1118af9b3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5b1997fb-8114-417a-a20b-796df5612ac9" xmlns:ns4="eefc82e4-fec2-46ce-83e1-5271053f7c9b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bb3db480e9256d19dbc0add7ebf3b44" ns3:_="" ns4:_="">
     <xsd:import namespace="5b1997fb-8114-417a-a20b-796df5612ac9"/>
@@ -1666,15 +1711,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1682,6 +1718,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19232968-D0AD-4578-90F9-FB7793DCA679}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24CD1E4A-6B0F-4C5B-8CAD-007A87F29157}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1696,14 +1740,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19232968-D0AD-4578-90F9-FB7793DCA679}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Changes made to Database XLS, new cities added
</commit_message>
<xml_diff>
--- a/DatabaseCitys.xlsx
+++ b/DatabaseCitys.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fn24x\CAMMM-Web-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB8E6F3-1F43-439B-BEF7-711B7724D603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20E2AFF-E3BB-43CC-8F92-13CE24BFD472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9210" yWindow="-4570" windowWidth="14850" windowHeight="9180" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
+    <workbookView xWindow="20770" yWindow="-3690" windowWidth="14850" windowHeight="9180" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="191028" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
   <si>
     <t>City</t>
   </si>
@@ -283,6 +283,36 @@
   </si>
   <si>
     <t>flags/hungary-flag-xs.png</t>
+  </si>
+  <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>https://www.mbta.com/developers/gtfs</t>
+  </si>
+  <si>
+    <t>flags/united-states-of-america-flag-xs.png</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Longueuil</t>
+  </si>
+  <si>
+    <t>Vancouver</t>
+  </si>
+  <si>
+    <t>GTA</t>
+  </si>
+  <si>
+    <t>https://open.toronto.ca/dataset/ttc-routes-and-schedules/</t>
+  </si>
+  <si>
+    <t>https://www.rtl-longueuil.qc.ca/en-CA/open-data/gtfs-files/</t>
+  </si>
+  <si>
+    <t>https://developer.translink.ca/servicesgtfs/gtfsdata</t>
   </si>
 </sst>
 </file>
@@ -333,7 +363,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -354,6 +384,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -674,11 +707,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E70725-99F3-4F19-8F96-434E9A453C7B}">
-  <dimension ref="A1:AM10"/>
+  <dimension ref="A1:AM11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2610" topLeftCell="AJ1" activePane="topRight"/>
-      <selection pane="topRight" activeCell="AM7" sqref="AM7"/>
+      <pane xSplit="2620" topLeftCell="AJ1" activePane="topRight"/>
+      <selection activeCell="B9" sqref="B9"/>
+      <selection pane="topRight" activeCell="AM12" sqref="AM12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -716,108 +750,108 @@
     <col min="36" max="36" width="19.33203125" style="1" customWidth="1"/>
     <col min="37" max="37" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="30.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="36.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="40" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="9"/>
+      <c r="G1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8" t="s">
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8" t="s">
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8" t="s">
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8" t="s">
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AE1" s="8" t="s">
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AE1" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AF1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AG1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH1" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AI1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AJ1" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AK1" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AL1" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AM1" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
       <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
@@ -881,15 +915,15 @@
       <c r="AD2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="8"/>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="8"/>
-      <c r="AK2" s="8"/>
-      <c r="AL2" s="8"/>
-      <c r="AM2" s="8"/>
+      <c r="AE2" s="9"/>
+      <c r="AF2" s="9"/>
+      <c r="AG2" s="9"/>
+      <c r="AH2" s="9"/>
+      <c r="AI2" s="9"/>
+      <c r="AJ2" s="9"/>
+      <c r="AK2" s="9"/>
+      <c r="AL2" s="9"/>
+      <c r="AM2" s="9"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1452,11 +1486,340 @@
         <v>79</v>
       </c>
     </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H8" s="3">
+        <v>4</v>
+      </c>
+      <c r="K8" s="1">
+        <v>7460</v>
+      </c>
+      <c r="L8" s="1">
+        <v>170</v>
+      </c>
+      <c r="M8" s="1">
+        <v>267</v>
+      </c>
+      <c r="O8" s="1">
+        <v>129</v>
+      </c>
+      <c r="P8" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>3533</v>
+      </c>
+      <c r="S8" s="1">
+        <v>46</v>
+      </c>
+      <c r="T8" s="1">
+        <v>13</v>
+      </c>
+      <c r="U8" s="1">
+        <v>675</v>
+      </c>
+      <c r="W8" s="1">
+        <v>98</v>
+      </c>
+      <c r="X8" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>643</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>23</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>232.11</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>5396</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>2021</v>
+      </c>
+      <c r="AI8" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="AJ8" s="1">
+        <v>2022</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3</v>
+      </c>
+      <c r="K9" s="1">
+        <v>26746</v>
+      </c>
+      <c r="L9" s="1">
+        <v>476</v>
+      </c>
+      <c r="M9" s="1">
+        <v>11963</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1">
+        <v>140</v>
+      </c>
+      <c r="T9" s="1">
+        <v>4</v>
+      </c>
+      <c r="U9" s="1">
+        <v>904</v>
+      </c>
+      <c r="W9" s="1">
+        <v>866</v>
+      </c>
+      <c r="X9" s="1">
+        <v>13</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>15509</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>27</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>7123.64</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>6.71</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>942</v>
+      </c>
+      <c r="AH9" s="1">
+        <v>2020</v>
+      </c>
+      <c r="AI9" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="AJ9" s="1">
+        <v>2022</v>
+      </c>
+      <c r="AM9" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
     <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="K10" s="1">
+        <v>6171</v>
+      </c>
+      <c r="L10" s="1">
+        <v>153</v>
+      </c>
+      <c r="M10" s="1">
+        <v>302</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
+      <c r="U10" s="1">
+        <v>0</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0</v>
+      </c>
+      <c r="X10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>122.9</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>2002</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>2016</v>
+      </c>
+      <c r="AI10" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="AJ10" s="1">
+        <v>2022</v>
+      </c>
       <c r="AL10" s="7"/>
+      <c r="AM10" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2</v>
+      </c>
+      <c r="K11" s="1">
+        <v>13299</v>
+      </c>
+      <c r="L11" s="1">
+        <v>232</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1359</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="S11" s="1">
+        <v>70</v>
+      </c>
+      <c r="T11" s="1">
+        <v>3</v>
+      </c>
+      <c r="U11" s="1">
+        <v>5325</v>
+      </c>
+      <c r="W11" s="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>22</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>2878.52</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>2.64</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>2584</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>2016</v>
+      </c>
+      <c r="AI11" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>2022</v>
+      </c>
+      <c r="AM11" s="8" t="s">
+        <v>79</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="AM1:AM2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="AG1:AG2"/>
@@ -1465,23 +1828,18 @@
     <mergeCell ref="Z1:AC1"/>
     <mergeCell ref="AK1:AK2"/>
     <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="E1:F1"/>
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
     <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="AE1:AE2"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="AI8" r:id="rId1" tooltip="https://www.mbta.com/developers/gtfs" xr:uid="{497ED0E1-F448-4551-9FBE-9383EC70C3AD}"/>
+    <hyperlink ref="AI9" r:id="rId2" xr:uid="{521D9DA3-49D7-48A9-AE52-2CF4691F020B}"/>
+    <hyperlink ref="AI10" r:id="rId3" xr:uid="{530467A5-85B4-48A0-9CC2-294744E30FF7}"/>
+    <hyperlink ref="AI11" r:id="rId4" tooltip="https://developer.translink.ca/servicesgtfs/gtfsdata" xr:uid="{22E1B776-E695-4EC3-9347-30987D601125}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId5"/>
 </worksheet>
 </file>
 
@@ -1495,6 +1853,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BFE9A4688917F64EA5EF44A4A73B6A0B" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1d0e5df5db596ad1f7ae9b1118af9b3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5b1997fb-8114-417a-a20b-796df5612ac9" xmlns:ns4="eefc82e4-fec2-46ce-83e1-5271053f7c9b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bb3db480e9256d19dbc0add7ebf3b44" ns3:_="" ns4:_="">
     <xsd:import namespace="5b1997fb-8114-417a-a20b-796df5612ac9"/>
@@ -1711,12 +2075,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19232968-D0AD-4578-90F9-FB7793DCA679}">
   <ds:schemaRefs>
@@ -1726,6 +2084,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99010E58-C46F-4EC0-AEBC-FB07528535B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="5b1997fb-8114-417a-a20b-796df5612ac9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="eefc82e4-fec2-46ce-83e1-5271053f7c9b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24CD1E4A-6B0F-4C5B-8CAD-007A87F29157}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1742,21 +2117,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99010E58-C46F-4EC0-AEBC-FB07528535B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="5b1997fb-8114-417a-a20b-796df5612ac9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="eefc82e4-fec2-46ce-83e1-5271053f7c9b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update to the DataCities excel
Update to the DataCities excel
</commit_message>
<xml_diff>
--- a/DatabaseCitys.xlsx
+++ b/DatabaseCitys.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fn24x\CAMMM-Web-Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\GitTesting\CAMMM-Web-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B20E2AFF-E3BB-43CC-8F92-13CE24BFD472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164288BA-E6F3-4030-B487-023E0B6C6C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20770" yWindow="-3690" windowWidth="14850" windowHeight="9180" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
+    <workbookView xWindow="10245" yWindow="4965" windowWidth="18210" windowHeight="9795" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -207,9 +207,6 @@
     <t>Wien</t>
   </si>
   <si>
-    <t>ckv8617pd0n9g14rxpi45ts4u</t>
-  </si>
-  <si>
     <t>YearOfStats</t>
   </si>
   <si>
@@ -246,30 +243,18 @@
     <t>montreal_grid</t>
   </si>
   <si>
-    <t>vienna_grid</t>
-  </si>
-  <si>
     <t>cl1qj5iio000h14lsrpfbbbs7</t>
   </si>
   <si>
     <t>cl1qjcbr9000e15s7ids0qcrt</t>
   </si>
   <si>
-    <t>barcelona_grid</t>
-  </si>
-  <si>
     <t>cl1qjqiij002h14s6sigeccvb</t>
   </si>
   <si>
-    <t>budapest_grid</t>
-  </si>
-  <si>
     <t>cl1qjjphy000g15s7jf1t62sy</t>
   </si>
   <si>
-    <t>quebec_grid</t>
-  </si>
-  <si>
     <t>Flag</t>
   </si>
   <si>
@@ -313,13 +298,28 @@
   </si>
   <si>
     <t>https://developer.translink.ca/servicesgtfs/gtfsdata</t>
+  </si>
+  <si>
+    <t>quebec-grid</t>
+  </si>
+  <si>
+    <t>budapest-grid</t>
+  </si>
+  <si>
+    <t>barcelona-grid</t>
+  </si>
+  <si>
+    <t>vienna-grid</t>
+  </si>
+  <si>
+    <t>ckv86yukx9ah014qmn2khc2kc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,6 +337,19 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9AA5CE"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -363,7 +376,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -390,6 +403,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -710,148 +732,148 @@
   <dimension ref="A1:AM11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2620" topLeftCell="AJ1" activePane="topRight"/>
-      <selection activeCell="B9" sqref="B9"/>
-      <selection pane="topRight" activeCell="AM12" sqref="AM12"/>
+      <pane xSplit="2625" topLeftCell="B1" activePane="topRight"/>
+      <selection sqref="A1:A2"/>
+      <selection pane="topRight" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.44140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="32.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="40.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="26" width="9.109375" style="1"/>
-    <col min="27" max="27" width="13.44140625" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11.5546875" style="1" customWidth="1"/>
-    <col min="29" max="29" width="11.88671875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="32.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="40.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="9.140625" style="1"/>
+    <col min="27" max="27" width="13.42578125" style="1" customWidth="1"/>
+    <col min="28" max="28" width="11.5703125" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11.85546875" style="1" customWidth="1"/>
     <col min="30" max="30" width="15" style="1" customWidth="1"/>
-    <col min="31" max="31" width="9.109375" style="1"/>
-    <col min="32" max="32" width="13.44140625" style="1" customWidth="1"/>
-    <col min="33" max="33" width="12.5546875" style="1" customWidth="1"/>
-    <col min="34" max="34" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="70.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.33203125" style="1" customWidth="1"/>
-    <col min="37" max="37" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="30.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="36.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="9.109375" style="1"/>
+    <col min="31" max="31" width="9.140625" style="1"/>
+    <col min="32" max="32" width="13.42578125" style="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5703125" style="1" customWidth="1"/>
+    <col min="34" max="34" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="70.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.28515625" style="1" customWidth="1"/>
+    <col min="37" max="37" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="30.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="36.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9" t="s">
+      <c r="F1" s="10"/>
+      <c r="G1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H1" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9" t="s">
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9" t="s">
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9" t="s">
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9" t="s">
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AE1" s="9" t="s">
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
+      <c r="AC1" s="10"/>
+      <c r="AE1" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AF1" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AG1" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AH1" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="AI1" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="AI1" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="AK1" s="9" t="s">
+      <c r="AJ1" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK1" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AL1" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="AL1" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="AM1" s="9" t="s">
-        <v>78</v>
+      <c r="AM1" s="10" t="s">
+        <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A2" s="9"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="9"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="10"/>
       <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
@@ -915,17 +937,17 @@
       <c r="AD2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="9"/>
-      <c r="AF2" s="9"/>
-      <c r="AG2" s="9"/>
-      <c r="AH2" s="9"/>
-      <c r="AI2" s="9"/>
-      <c r="AJ2" s="9"/>
-      <c r="AK2" s="9"/>
-      <c r="AL2" s="9"/>
-      <c r="AM2" s="9"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="10"/>
+      <c r="AM2" s="10"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1021,22 +1043,22 @@
         <v>2016</v>
       </c>
       <c r="AI3" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AJ3" s="1">
         <v>2021</v>
       </c>
       <c r="AK3" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AL3" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AM3" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1135,22 +1157,22 @@
         <v>2019</v>
       </c>
       <c r="AI4" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AJ4" s="5">
         <v>2021</v>
       </c>
       <c r="AK4" s="6" t="s">
-        <v>70</v>
+        <v>91</v>
       </c>
       <c r="AL4" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="AM4" s="1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1246,22 +1268,22 @@
         <v>2015</v>
       </c>
       <c r="AI5" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AJ5" s="5">
         <v>2021</v>
       </c>
       <c r="AK5" s="6" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="AL5" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="AM5" s="1" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
@@ -1363,30 +1385,30 @@
         <v>2014</v>
       </c>
       <c r="AI6" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AJ6" s="5">
         <v>2021</v>
       </c>
       <c r="AK6" s="6" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="AL6" s="6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="AM6" s="1" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>57</v>
+      <c r="C7" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>52</v>
@@ -1471,28 +1493,30 @@
         <v>2016</v>
       </c>
       <c r="AI7" s="5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AJ7" s="5">
         <v>2021</v>
       </c>
       <c r="AK7" s="6" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="AL7" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="AM7" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>83</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="11"/>
       <c r="H8" s="3">
         <v>4</v>
       </c>
@@ -1557,21 +1581,21 @@
         <v>2021</v>
       </c>
       <c r="AI8" s="8" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="AJ8" s="1">
         <v>2022</v>
       </c>
       <c r="AM8" s="1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="H9" s="3">
         <v>3</v>
@@ -1637,21 +1661,21 @@
         <v>2020</v>
       </c>
       <c r="AI9" s="8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="AJ9" s="1">
         <v>2022</v>
       </c>
       <c r="AM9" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="H10" s="3">
         <v>1</v>
@@ -1717,22 +1741,22 @@
         <v>2016</v>
       </c>
       <c r="AI10" s="8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="AJ10" s="1">
         <v>2022</v>
       </c>
       <c r="AL10" s="7"/>
       <c r="AM10" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="H11" s="3">
         <v>2</v>
@@ -1798,17 +1822,28 @@
         <v>2016</v>
       </c>
       <c r="AI11" s="8" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="AJ11" s="1">
         <v>2022</v>
       </c>
       <c r="AM11" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="AM1:AM2"/>
+    <mergeCell ref="AF1:AF2"/>
+    <mergeCell ref="AG1:AG2"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:Y1"/>
+    <mergeCell ref="Z1:AC1"/>
+    <mergeCell ref="AK1:AK2"/>
+    <mergeCell ref="AL1:AL2"/>
+    <mergeCell ref="AH1:AH2"/>
+    <mergeCell ref="AI1:AI2"/>
+    <mergeCell ref="AJ1:AJ2"/>
     <mergeCell ref="J1:M1"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="AE1:AE2"/>
@@ -1820,17 +1855,6 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:F1"/>
-    <mergeCell ref="AM1:AM2"/>
-    <mergeCell ref="AF1:AF2"/>
-    <mergeCell ref="AG1:AG2"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:Y1"/>
-    <mergeCell ref="Z1:AC1"/>
-    <mergeCell ref="AK1:AK2"/>
-    <mergeCell ref="AL1:AL2"/>
-    <mergeCell ref="AH1:AH2"/>
-    <mergeCell ref="AI1:AI2"/>
-    <mergeCell ref="AJ1:AJ2"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AI8" r:id="rId1" tooltip="https://www.mbta.com/developers/gtfs" xr:uid="{497ED0E1-F448-4551-9FBE-9383EC70C3AD}"/>
@@ -1844,18 +1868,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2076,14 +2100,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19232968-D0AD-4578-90F9-FB7793DCA679}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99010E58-C46F-4EC0-AEBC-FB07528535B3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -2096,6 +2112,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="eefc82e4-fec2-46ce-83e1-5271053f7c9b"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19232968-D0AD-4578-90F9-FB7793DCA679}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fixed refactoring of infopopups and added grid layers
</commit_message>
<xml_diff>
--- a/DatabaseCitys.xlsx
+++ b/DatabaseCitys.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\GitTesting\CAMMM-Web-Tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fn24x\CAMMM-Web-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164288BA-E6F3-4030-B487-023E0B6C6C30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F4E72A-D376-495A-A636-52E4BDFCA1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10245" yWindow="4965" windowWidth="18210" windowHeight="9795" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
+    <workbookView xWindow="20770" yWindow="-3690" windowWidth="17820" windowHeight="11020" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
   <si>
     <t>City</t>
   </si>
@@ -270,56 +270,26 @@
     <t>flags/hungary-flag-xs.png</t>
   </si>
   <si>
-    <t>Boston</t>
-  </si>
-  <si>
-    <t>https://www.mbta.com/developers/gtfs</t>
-  </si>
-  <si>
-    <t>flags/united-states-of-america-flag-xs.png</t>
-  </si>
-  <si>
-    <t>Toronto</t>
-  </si>
-  <si>
-    <t>Longueuil</t>
-  </si>
-  <si>
-    <t>Vancouver</t>
-  </si>
-  <si>
-    <t>GTA</t>
-  </si>
-  <si>
-    <t>https://open.toronto.ca/dataset/ttc-routes-and-schedules/</t>
-  </si>
-  <si>
-    <t>https://www.rtl-longueuil.qc.ca/en-CA/open-data/gtfs-files/</t>
-  </si>
-  <si>
-    <t>https://developer.translink.ca/servicesgtfs/gtfsdata</t>
-  </si>
-  <si>
-    <t>quebec-grid</t>
-  </si>
-  <si>
-    <t>budapest-grid</t>
-  </si>
-  <si>
-    <t>barcelona-grid</t>
-  </si>
-  <si>
-    <t>vienna-grid</t>
-  </si>
-  <si>
     <t>ckv86yukx9ah014qmn2khc2kc</t>
+  </si>
+  <si>
+    <t>vienna_grid</t>
+  </si>
+  <si>
+    <t>barcelona_grid</t>
+  </si>
+  <si>
+    <t>budapest_grid</t>
+  </si>
+  <si>
+    <t>quebec_grid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -328,27 +298,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9AA5CE"/>
-      <name val="Consolas"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <strike/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -372,11 +321,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -396,27 +344,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -729,151 +664,151 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E70725-99F3-4F19-8F96-434E9A453C7B}">
-  <dimension ref="A1:AM11"/>
+  <dimension ref="A1:AM7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2625" topLeftCell="B1" activePane="topRight"/>
-      <selection sqref="A1:A2"/>
-      <selection pane="topRight" activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane xSplit="2620" topLeftCell="AI1" activePane="topRight"/>
+      <selection activeCell="C14" sqref="C14"/>
+      <selection pane="topRight" activeCell="AK3" sqref="AK3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="30.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="31.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="13.42578125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="32.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="37.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="40.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="26" width="9.140625" style="1"/>
-    <col min="27" max="27" width="13.42578125" style="1" customWidth="1"/>
-    <col min="28" max="28" width="11.5703125" style="1" customWidth="1"/>
-    <col min="29" max="29" width="11.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="13.44140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="32.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="37.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="40.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="26" width="9.109375" style="1"/>
+    <col min="27" max="27" width="13.44140625" style="1" customWidth="1"/>
+    <col min="28" max="28" width="11.5546875" style="1" customWidth="1"/>
+    <col min="29" max="29" width="11.88671875" style="1" customWidth="1"/>
     <col min="30" max="30" width="15" style="1" customWidth="1"/>
-    <col min="31" max="31" width="9.140625" style="1"/>
-    <col min="32" max="32" width="13.42578125" style="1" customWidth="1"/>
-    <col min="33" max="33" width="12.5703125" style="1" customWidth="1"/>
-    <col min="34" max="34" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="70.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="19.28515625" style="1" customWidth="1"/>
-    <col min="37" max="37" width="31.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="30.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="36.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="16384" width="9.140625" style="1"/>
+    <col min="31" max="31" width="9.109375" style="1"/>
+    <col min="32" max="32" width="13.44140625" style="1" customWidth="1"/>
+    <col min="33" max="33" width="12.5546875" style="1" customWidth="1"/>
+    <col min="34" max="34" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="70.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.33203125" style="1" customWidth="1"/>
+    <col min="37" max="37" width="31.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="30.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="36.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10" t="s">
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="J1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10" t="s">
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10" t="s">
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10" t="s">
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10" t="s">
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AE1" s="10" t="s">
+      <c r="AA1" s="8"/>
+      <c r="AB1" s="8"/>
+      <c r="AC1" s="8"/>
+      <c r="AE1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="10" t="s">
+      <c r="AF1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="10" t="s">
+      <c r="AG1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="10" t="s">
+      <c r="AH1" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="10" t="s">
+      <c r="AI1" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="AJ1" s="10" t="s">
+      <c r="AJ1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="AK1" s="10" t="s">
+      <c r="AK1" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="AL1" s="10" t="s">
+      <c r="AL1" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="AM1" s="10" t="s">
+      <c r="AM1" s="8" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A2" s="10"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
+    <row r="2" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
       <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
@@ -937,17 +872,17 @@
       <c r="AD2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AH2" s="10"/>
-      <c r="AI2" s="10"/>
-      <c r="AJ2" s="10"/>
-      <c r="AK2" s="10"/>
-      <c r="AL2" s="10"/>
-      <c r="AM2" s="10"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>23</v>
       </c>
@@ -1058,7 +993,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>30</v>
       </c>
@@ -1163,7 +1098,7 @@
         <v>2021</v>
       </c>
       <c r="AK4" s="6" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="AL4" s="6" t="s">
         <v>69</v>
@@ -1172,7 +1107,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -1274,7 +1209,7 @@
         <v>2021</v>
       </c>
       <c r="AK5" s="6" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="AL5" s="6" t="s">
         <v>70</v>
@@ -1283,7 +1218,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>43</v>
       </c>
@@ -1391,7 +1326,7 @@
         <v>2021</v>
       </c>
       <c r="AK6" s="6" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="AL6" s="6" t="s">
         <v>71</v>
@@ -1400,15 +1335,15 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>92</v>
+      <c r="C7" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>52</v>
@@ -1499,335 +1434,12 @@
         <v>2021</v>
       </c>
       <c r="AK7" s="6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="AL7" s="6" t="s">
         <v>72</v>
       </c>
       <c r="AM7" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="11"/>
-      <c r="H8" s="3">
-        <v>4</v>
-      </c>
-      <c r="K8" s="1">
-        <v>7460</v>
-      </c>
-      <c r="L8" s="1">
-        <v>170</v>
-      </c>
-      <c r="M8" s="1">
-        <v>267</v>
-      </c>
-      <c r="O8" s="1">
-        <v>129</v>
-      </c>
-      <c r="P8" s="1">
-        <v>12</v>
-      </c>
-      <c r="Q8" s="1">
-        <v>3533</v>
-      </c>
-      <c r="S8" s="1">
-        <v>46</v>
-      </c>
-      <c r="T8" s="1">
-        <v>13</v>
-      </c>
-      <c r="U8" s="1">
-        <v>675</v>
-      </c>
-      <c r="W8" s="1">
-        <v>98</v>
-      </c>
-      <c r="X8" s="1">
-        <v>5</v>
-      </c>
-      <c r="Y8" s="1">
-        <v>643</v>
-      </c>
-      <c r="AA8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="1">
-        <v>23</v>
-      </c>
-      <c r="AE8" s="1">
-        <v>232.11</v>
-      </c>
-      <c r="AF8" s="1">
-        <v>4.9400000000000004</v>
-      </c>
-      <c r="AG8" s="1">
-        <v>5396</v>
-      </c>
-      <c r="AH8" s="1">
-        <v>2021</v>
-      </c>
-      <c r="AI8" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="AJ8" s="1">
-        <v>2022</v>
-      </c>
-      <c r="AM8" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="H9" s="3">
-        <v>3</v>
-      </c>
-      <c r="K9" s="1">
-        <v>26746</v>
-      </c>
-      <c r="L9" s="1">
-        <v>476</v>
-      </c>
-      <c r="M9" s="1">
-        <v>11963</v>
-      </c>
-      <c r="O9" s="1">
-        <v>0</v>
-      </c>
-      <c r="P9" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>0</v>
-      </c>
-      <c r="S9" s="1">
-        <v>140</v>
-      </c>
-      <c r="T9" s="1">
-        <v>4</v>
-      </c>
-      <c r="U9" s="1">
-        <v>904</v>
-      </c>
-      <c r="W9" s="1">
-        <v>866</v>
-      </c>
-      <c r="X9" s="1">
-        <v>13</v>
-      </c>
-      <c r="Y9" s="1">
-        <v>15509</v>
-      </c>
-      <c r="AA9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="1">
-        <v>27</v>
-      </c>
-      <c r="AE9" s="1">
-        <v>7123.64</v>
-      </c>
-      <c r="AF9" s="1">
-        <v>6.71</v>
-      </c>
-      <c r="AG9" s="1">
-        <v>942</v>
-      </c>
-      <c r="AH9" s="1">
-        <v>2020</v>
-      </c>
-      <c r="AI9" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="AJ9" s="1">
-        <v>2022</v>
-      </c>
-      <c r="AM9" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="H10" s="3">
-        <v>1</v>
-      </c>
-      <c r="K10" s="1">
-        <v>6171</v>
-      </c>
-      <c r="L10" s="1">
-        <v>153</v>
-      </c>
-      <c r="M10" s="1">
-        <v>302</v>
-      </c>
-      <c r="O10" s="1">
-        <v>0</v>
-      </c>
-      <c r="P10" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="1">
-        <v>0</v>
-      </c>
-      <c r="S10" s="1">
-        <v>0</v>
-      </c>
-      <c r="T10" s="1">
-        <v>0</v>
-      </c>
-      <c r="U10" s="1">
-        <v>0</v>
-      </c>
-      <c r="W10" s="1">
-        <v>0</v>
-      </c>
-      <c r="X10" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="1">
-        <v>4</v>
-      </c>
-      <c r="AE10" s="1">
-        <v>122.9</v>
-      </c>
-      <c r="AF10" s="1">
-        <v>0.23</v>
-      </c>
-      <c r="AG10" s="1">
-        <v>2002</v>
-      </c>
-      <c r="AH10" s="1">
-        <v>2016</v>
-      </c>
-      <c r="AI10" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="AJ10" s="1">
-        <v>2022</v>
-      </c>
-      <c r="AL10" s="7"/>
-      <c r="AM10" s="8" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H11" s="3">
-        <v>2</v>
-      </c>
-      <c r="K11" s="1">
-        <v>13299</v>
-      </c>
-      <c r="L11" s="1">
-        <v>232</v>
-      </c>
-      <c r="M11" s="1">
-        <v>1359</v>
-      </c>
-      <c r="O11" s="1">
-        <v>0</v>
-      </c>
-      <c r="P11" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="1">
-        <v>0</v>
-      </c>
-      <c r="S11" s="1">
-        <v>70</v>
-      </c>
-      <c r="T11" s="1">
-        <v>3</v>
-      </c>
-      <c r="U11" s="1">
-        <v>5325</v>
-      </c>
-      <c r="W11" s="1">
-        <v>0</v>
-      </c>
-      <c r="X11" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="1">
-        <v>22</v>
-      </c>
-      <c r="AE11" s="1">
-        <v>2878.52</v>
-      </c>
-      <c r="AF11" s="1">
-        <v>2.64</v>
-      </c>
-      <c r="AG11" s="1">
-        <v>2584</v>
-      </c>
-      <c r="AH11" s="1">
-        <v>2016</v>
-      </c>
-      <c r="AI11" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="AJ11" s="1">
-        <v>2022</v>
-      </c>
-      <c r="AM11" s="8" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1856,24 +1468,12 @@
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="E1:F1"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="AI8" r:id="rId1" tooltip="https://www.mbta.com/developers/gtfs" xr:uid="{497ED0E1-F448-4551-9FBE-9383EC70C3AD}"/>
-    <hyperlink ref="AI9" r:id="rId2" xr:uid="{521D9DA3-49D7-48A9-AE52-2CF4691F020B}"/>
-    <hyperlink ref="AI10" r:id="rId3" xr:uid="{530467A5-85B4-48A0-9CC2-294744E30FF7}"/>
-    <hyperlink ref="AI11" r:id="rId4" tooltip="https://developer.translink.ca/servicesgtfs/gtfsdata" xr:uid="{22E1B776-E695-4EC3-9347-30987D601125}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -1882,7 +1482,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BFE9A4688917F64EA5EF44A4A73B6A0B" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1d0e5df5db596ad1f7ae9b1118af9b3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5b1997fb-8114-417a-a20b-796df5612ac9" xmlns:ns4="eefc82e4-fec2-46ce-83e1-5271053f7c9b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bb3db480e9256d19dbc0add7ebf3b44" ns3:_="" ns4:_="">
     <xsd:import namespace="5b1997fb-8114-417a-a20b-796df5612ac9"/>
@@ -2099,24 +1699,13 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99010E58-C46F-4EC0-AEBC-FB07528535B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="5b1997fb-8114-417a-a20b-796df5612ac9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="eefc82e4-fec2-46ce-83e1-5271053f7c9b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19232968-D0AD-4578-90F9-FB7793DCA679}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -2124,7 +1713,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24CD1E4A-6B0F-4C5B-8CAD-007A87F29157}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2141,4 +1730,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99010E58-C46F-4EC0-AEBC-FB07528535B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="5b1997fb-8114-417a-a20b-796df5612ac9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="eefc82e4-fec2-46ce-83e1-5271053f7c9b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated to 11 cities
Co-authored-by: Omar Ortiz Meraz <omar.ortizmeraz@mail.concordia.ca>
</commit_message>
<xml_diff>
--- a/DatabaseCitys.xlsx
+++ b/DatabaseCitys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fn24x\CAMMM-Web-Tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03F4E72A-D376-495A-A636-52E4BDFCA1F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{779C529E-7D21-4CAE-B796-7DB7E12BFCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20770" yWindow="-3690" windowWidth="17820" windowHeight="11020" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
+    <workbookView xWindow="13500" yWindow="-2180" windowWidth="17820" windowHeight="11020" xr2:uid="{F6B95E2D-C01D-4376-BFCA-1DC2F1C9A821}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="135">
   <si>
     <t>City</t>
   </si>
@@ -270,9 +270,57 @@
     <t>flags/hungary-flag-xs.png</t>
   </si>
   <si>
+    <t>Boston</t>
+  </si>
+  <si>
+    <t>https://www.mbta.com/developers/gtfs</t>
+  </si>
+  <si>
+    <t>flags/united-states-of-america-flag-xs.png</t>
+  </si>
+  <si>
+    <t>Toronto</t>
+  </si>
+  <si>
+    <t>Longueuil</t>
+  </si>
+  <si>
+    <t>Vancouver</t>
+  </si>
+  <si>
+    <t>GTA</t>
+  </si>
+  <si>
+    <t>https://open.toronto.ca/dataset/ttc-routes-and-schedules/</t>
+  </si>
+  <si>
+    <t>https://www.rtl-longueuil.qc.ca/en-CA/open-data/gtfs-files/</t>
+  </si>
+  <si>
+    <t>https://developer.translink.ca/servicesgtfs/gtfsdata</t>
+  </si>
+  <si>
     <t>ckv86yukx9ah014qmn2khc2kc</t>
   </si>
   <si>
+    <t>cl2j3s9ml000514p2mejx0yqb</t>
+  </si>
+  <si>
+    <t>boston_N_CD,  boston_N_CL</t>
+  </si>
+  <si>
+    <t>boston-bus_CD, boston-bus_CL</t>
+  </si>
+  <si>
+    <t>boston-rail_CD, boston-rail_CL</t>
+  </si>
+  <si>
+    <t>boston-metro_CD, boston-metro_CL</t>
+  </si>
+  <si>
+    <t>boston-lightrail_CD, boston-lightrail_CL</t>
+  </si>
+  <si>
     <t>vienna_grid</t>
   </si>
   <si>
@@ -283,13 +331,121 @@
   </si>
   <si>
     <t>quebec_grid</t>
+  </si>
+  <si>
+    <t>boston_grid</t>
+  </si>
+  <si>
+    <t>longueuil_grid</t>
+  </si>
+  <si>
+    <t>cl2j3s9zm000h14nx6x271uo1</t>
+  </si>
+  <si>
+    <t>longueuil-bus_CD, longueuil-bus_CL</t>
+  </si>
+  <si>
+    <t>cl2j5m6qv000l14ltq66brxkm</t>
+  </si>
+  <si>
+    <t>longueuil_N_CD, longueuil_N_CL</t>
+  </si>
+  <si>
+    <t>cl2j761fv000z14oybd9dv087</t>
+  </si>
+  <si>
+    <t>vancouver-bus_CD, vancouver-bus_CL</t>
+  </si>
+  <si>
+    <t>vancouver-metro_CD, vancouver-metro_CL</t>
+  </si>
+  <si>
+    <t>vancouver_grid</t>
+  </si>
+  <si>
+    <t>cl2j7dxy7001114oy0fwtufye</t>
+  </si>
+  <si>
+    <t>vancouver_N_CD, vancouver_N_CL</t>
+  </si>
+  <si>
+    <t>cl2j65p95000l14qh59j99qq7</t>
+  </si>
+  <si>
+    <t>cl2jkjtrb004n14mt0ew9jj0v</t>
+  </si>
+  <si>
+    <t>toronto-bus_CD, toronto-bus_CL</t>
+  </si>
+  <si>
+    <t>toronto_N_CD, toronto_N_CL</t>
+  </si>
+  <si>
+    <t>cl2jhcd6z001l15ogcoitd1zj</t>
+  </si>
+  <si>
+    <t>toronto-metro_CD, toronto-metro_CL</t>
+  </si>
+  <si>
+    <t>toronto-lightrail_CD, toronto-lightrail_CL</t>
+  </si>
+  <si>
+    <t>toronto_grid</t>
+  </si>
+  <si>
+    <t>Laval</t>
+  </si>
+  <si>
+    <t>cl2jhkvs9000215nt1rjl6mrv</t>
+  </si>
+  <si>
+    <t>cl2jk6kpl002e14sabu3e2gpu</t>
+  </si>
+  <si>
+    <t>laval_grid</t>
+  </si>
+  <si>
+    <t>laval_N_CD, laval_N_CL</t>
+  </si>
+  <si>
+    <t>Seattle</t>
+  </si>
+  <si>
+    <t>laval-bus_CD, laval-bus_CL</t>
+  </si>
+  <si>
+    <t>cl2jfqz27000l15se1zk59igu</t>
+  </si>
+  <si>
+    <t>cl2jgv5qs004b14mtorc476ks</t>
+  </si>
+  <si>
+    <t>seattle_N_CD,seattle_N_CD</t>
+  </si>
+  <si>
+    <t>seattle-bus_CD, seattle-bus_CL</t>
+  </si>
+  <si>
+    <t>seattle-rail_CD, seattle-rail_CL</t>
+  </si>
+  <si>
+    <t>seattle-lightrail_CD, seattle-lightrail_CL</t>
+  </si>
+  <si>
+    <t>seattle_grid</t>
+  </si>
+  <si>
+    <t>https://stlaval.ca/a-propos/diffusion/donnees-ouvertes</t>
+  </si>
+  <si>
+    <t>https://www.soundtransit.org/help-contacts/business-information/open-transit-data-otd/otd-downloads</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,6 +455,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -321,10 +485,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -344,6 +509,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -351,7 +534,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -664,12 +848,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E70725-99F3-4F19-8F96-434E9A453C7B}">
-  <dimension ref="A1:AM7"/>
+  <dimension ref="A1:AM13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane xSplit="2620" topLeftCell="AI1" activePane="topRight"/>
-      <selection activeCell="C14" sqref="C14"/>
-      <selection pane="topRight" activeCell="AK3" sqref="AK3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2630" activePane="topRight"/>
+      <selection activeCell="A13" sqref="A13"/>
+      <selection pane="topRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -677,8 +861,8 @@
     <col min="1" max="1" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -712,103 +896,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="8" t="s">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8" t="s">
+      <c r="F1" s="14"/>
+      <c r="G1" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8" t="s">
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8" t="s">
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8" t="s">
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8" t="s">
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AE1" s="8" t="s">
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AE1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="AF1" s="8" t="s">
+      <c r="AF1" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="AG1" s="8" t="s">
+      <c r="AG1" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="AH1" s="8" t="s">
+      <c r="AH1" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="AI1" s="8" t="s">
+      <c r="AI1" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="AJ1" s="8" t="s">
+      <c r="AJ1" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="AK1" s="8" t="s">
+      <c r="AK1" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="AL1" s="8" t="s">
+      <c r="AL1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="AM1" s="8" t="s">
+      <c r="AM1" s="14" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
       <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
       <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
@@ -872,15 +1056,15 @@
       <c r="AD2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AE2" s="8"/>
-      <c r="AF2" s="8"/>
-      <c r="AG2" s="8"/>
-      <c r="AH2" s="8"/>
-      <c r="AI2" s="8"/>
-      <c r="AJ2" s="8"/>
-      <c r="AK2" s="8"/>
-      <c r="AL2" s="8"/>
-      <c r="AM2" s="8"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14"/>
+      <c r="AH2" s="14"/>
+      <c r="AI2" s="14"/>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14"/>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="14"/>
     </row>
     <row r="3" spans="1:39" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -1098,7 +1282,7 @@
         <v>2021</v>
       </c>
       <c r="AK4" s="6" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="AL4" s="6" t="s">
         <v>69</v>
@@ -1209,7 +1393,7 @@
         <v>2021</v>
       </c>
       <c r="AK5" s="6" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="AL5" s="6" t="s">
         <v>70</v>
@@ -1326,7 +1510,7 @@
         <v>2021</v>
       </c>
       <c r="AK6" s="6" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="AL6" s="6" t="s">
         <v>71</v>
@@ -1342,8 +1526,8 @@
       <c r="B7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="7" t="s">
-        <v>78</v>
+      <c r="C7" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>52</v>
@@ -1434,17 +1618,669 @@
         <v>2021</v>
       </c>
       <c r="AK7" s="6" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="AL7" s="6" t="s">
         <v>72</v>
       </c>
       <c r="AM7" s="1" t="s">
         <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E8" s="12">
+        <v>-71.03</v>
+      </c>
+      <c r="F8" s="12">
+        <v>42.36</v>
+      </c>
+      <c r="G8" s="1">
+        <v>10.52</v>
+      </c>
+      <c r="H8" s="3">
+        <v>4</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="K8" s="1">
+        <v>7460</v>
+      </c>
+      <c r="L8" s="1">
+        <v>170</v>
+      </c>
+      <c r="M8" s="1">
+        <v>267</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="O8" s="1">
+        <v>129</v>
+      </c>
+      <c r="P8" s="1">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>3533</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="S8" s="1">
+        <v>46</v>
+      </c>
+      <c r="T8" s="1">
+        <v>13</v>
+      </c>
+      <c r="U8" s="1">
+        <v>675</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="W8" s="1">
+        <v>98</v>
+      </c>
+      <c r="X8" s="1">
+        <v>5</v>
+      </c>
+      <c r="Y8" s="1">
+        <v>643</v>
+      </c>
+      <c r="AA8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>23</v>
+      </c>
+      <c r="AE8" s="1">
+        <v>232.11</v>
+      </c>
+      <c r="AF8" s="1">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="AG8" s="1">
+        <v>5396</v>
+      </c>
+      <c r="AH8" s="1">
+        <v>2021</v>
+      </c>
+      <c r="AI8" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ8" s="1">
+        <v>2022</v>
+      </c>
+      <c r="AK8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="AM8" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E9" s="1">
+        <v>-79.400000000000006</v>
+      </c>
+      <c r="F9" s="1">
+        <v>43.63</v>
+      </c>
+      <c r="G9" s="1">
+        <v>9.1</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="J9" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="K9" s="1">
+        <v>26746</v>
+      </c>
+      <c r="L9" s="1">
+        <v>476</v>
+      </c>
+      <c r="M9" s="1">
+        <v>11963</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="S9" s="1">
+        <v>140</v>
+      </c>
+      <c r="T9" s="1">
+        <v>4</v>
+      </c>
+      <c r="U9" s="1">
+        <v>904</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="W9" s="1">
+        <v>866</v>
+      </c>
+      <c r="X9" s="1">
+        <v>13</v>
+      </c>
+      <c r="Y9" s="1">
+        <v>15509</v>
+      </c>
+      <c r="AA9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>27</v>
+      </c>
+      <c r="AE9" s="1">
+        <v>7123.64</v>
+      </c>
+      <c r="AF9" s="1">
+        <v>6.71</v>
+      </c>
+      <c r="AG9" s="1">
+        <v>942</v>
+      </c>
+      <c r="AH9" s="1">
+        <v>2020</v>
+      </c>
+      <c r="AI9" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="AJ9" s="1">
+        <v>2022</v>
+      </c>
+      <c r="AK9" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="AM9" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="E10" s="1">
+        <v>-73.44</v>
+      </c>
+      <c r="F10" s="12">
+        <v>45.52</v>
+      </c>
+      <c r="G10" s="1">
+        <v>12.22</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K10" s="1">
+        <v>6171</v>
+      </c>
+      <c r="L10" s="1">
+        <v>153</v>
+      </c>
+      <c r="M10" s="1">
+        <v>302</v>
+      </c>
+      <c r="O10" s="1">
+        <v>0</v>
+      </c>
+      <c r="P10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="1">
+        <v>0</v>
+      </c>
+      <c r="S10" s="1">
+        <v>0</v>
+      </c>
+      <c r="T10" s="1">
+        <v>0</v>
+      </c>
+      <c r="U10" s="1">
+        <v>0</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0</v>
+      </c>
+      <c r="X10" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="1">
+        <v>4</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>122.9</v>
+      </c>
+      <c r="AF10" s="1">
+        <v>0.23</v>
+      </c>
+      <c r="AG10" s="1">
+        <v>2002</v>
+      </c>
+      <c r="AH10" s="1">
+        <v>2016</v>
+      </c>
+      <c r="AI10" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="AJ10" s="1">
+        <v>2022</v>
+      </c>
+      <c r="AK10" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="AL10" s="7"/>
+      <c r="AM10" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="E11" s="1">
+        <v>-123.1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>49.223999999999997</v>
+      </c>
+      <c r="G11" s="1">
+        <v>10.98</v>
+      </c>
+      <c r="H11" s="3">
+        <v>2</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K11" s="1">
+        <v>13299</v>
+      </c>
+      <c r="L11" s="1">
+        <v>232</v>
+      </c>
+      <c r="M11" s="1">
+        <v>1359</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="1">
+        <v>0</v>
+      </c>
+      <c r="R11" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="S11" s="1">
+        <v>70</v>
+      </c>
+      <c r="T11" s="1">
+        <v>3</v>
+      </c>
+      <c r="U11" s="1">
+        <v>5325</v>
+      </c>
+      <c r="V11" s="11"/>
+      <c r="W11" s="1">
+        <v>0</v>
+      </c>
+      <c r="X11" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>22</v>
+      </c>
+      <c r="AE11" s="1">
+        <v>2878.52</v>
+      </c>
+      <c r="AF11" s="1">
+        <v>2.64</v>
+      </c>
+      <c r="AG11" s="1">
+        <v>2584</v>
+      </c>
+      <c r="AH11" s="1">
+        <v>2016</v>
+      </c>
+      <c r="AI11" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="AJ11" s="1">
+        <v>2022</v>
+      </c>
+      <c r="AK11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="AM11" s="8" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="1">
+        <v>-73.709999999999994</v>
+      </c>
+      <c r="F12" s="1">
+        <v>45.64</v>
+      </c>
+      <c r="G12" s="1">
+        <v>10.56</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K12" s="1">
+        <v>4910</v>
+      </c>
+      <c r="L12" s="1">
+        <v>50</v>
+      </c>
+      <c r="M12" s="1">
+        <v>714</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+      <c r="P12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="1">
+        <v>0</v>
+      </c>
+      <c r="S12" s="1">
+        <v>0</v>
+      </c>
+      <c r="T12" s="1">
+        <v>0</v>
+      </c>
+      <c r="U12" s="1">
+        <v>0</v>
+      </c>
+      <c r="W12" s="1">
+        <v>0</v>
+      </c>
+      <c r="X12" s="1">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="1">
+        <v>6</v>
+      </c>
+      <c r="AE12" s="1">
+        <v>247.23</v>
+      </c>
+      <c r="AF12" s="1">
+        <v>0.42</v>
+      </c>
+      <c r="AG12" s="1">
+        <v>1710</v>
+      </c>
+      <c r="AH12" s="1">
+        <v>2016</v>
+      </c>
+      <c r="AI12" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="AJ12" s="1">
+        <v>2022</v>
+      </c>
+      <c r="AK12" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="AM12" s="13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="E13" s="1">
+        <v>-122.22</v>
+      </c>
+      <c r="F13" s="1">
+        <v>47.5</v>
+      </c>
+      <c r="G13" s="1">
+        <v>9.2200000000000006</v>
+      </c>
+      <c r="H13" s="3">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="K13" s="1">
+        <v>13036</v>
+      </c>
+      <c r="M13" s="1">
+        <v>490</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="O13" s="1">
+        <v>11</v>
+      </c>
+      <c r="Q13" s="1">
+        <v>5891</v>
+      </c>
+      <c r="S13" s="1">
+        <v>0</v>
+      </c>
+      <c r="T13" s="1">
+        <v>0</v>
+      </c>
+      <c r="U13" s="1">
+        <v>0</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="W13" s="1">
+        <v>62</v>
+      </c>
+      <c r="Y13" s="1">
+        <v>8797</v>
+      </c>
+      <c r="AA13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="1">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="1">
+        <v>127</v>
+      </c>
+      <c r="AE13" s="1">
+        <v>21222</v>
+      </c>
+      <c r="AF13" s="1">
+        <v>4.01</v>
+      </c>
+      <c r="AG13" s="1">
+        <v>3387</v>
+      </c>
+      <c r="AH13" s="1">
+        <v>2019</v>
+      </c>
+      <c r="AI13" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="AJ13" s="1">
+        <v>2022</v>
+      </c>
+      <c r="AK13" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AM13" s="13" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="AE1:AE2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="E1:F1"/>
     <mergeCell ref="AM1:AM2"/>
     <mergeCell ref="AF1:AF2"/>
     <mergeCell ref="AG1:AG2"/>
@@ -1456,20 +2292,17 @@
     <mergeCell ref="AH1:AH2"/>
     <mergeCell ref="AI1:AI2"/>
     <mergeCell ref="AJ1:AJ2"/>
-    <mergeCell ref="J1:M1"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="AE1:AE2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="E1:F1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="AI8" r:id="rId1" tooltip="https://www.mbta.com/developers/gtfs" xr:uid="{497ED0E1-F448-4551-9FBE-9383EC70C3AD}"/>
+    <hyperlink ref="AI9" r:id="rId2" xr:uid="{521D9DA3-49D7-48A9-AE52-2CF4691F020B}"/>
+    <hyperlink ref="AI10" r:id="rId3" xr:uid="{530467A5-85B4-48A0-9CC2-294744E30FF7}"/>
+    <hyperlink ref="AI11" r:id="rId4" tooltip="https://developer.translink.ca/servicesgtfs/gtfsdata" xr:uid="{22E1B776-E695-4EC3-9347-30987D601125}"/>
+    <hyperlink ref="AI12" r:id="rId5" xr:uid="{4DCE1EE8-F904-4106-9523-730F596CD778}"/>
+    <hyperlink ref="AI13" r:id="rId6" xr:uid="{55B2FECF-74F4-43E3-A7AB-D4C4BFA907C5}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="1200" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -1483,6 +2316,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BFE9A4688917F64EA5EF44A4A73B6A0B" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1d0e5df5db596ad1f7ae9b1118af9b3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="5b1997fb-8114-417a-a20b-796df5612ac9" xmlns:ns4="eefc82e4-fec2-46ce-83e1-5271053f7c9b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6bb3db480e9256d19dbc0add7ebf3b44" ns3:_="" ns4:_="">
     <xsd:import namespace="5b1997fb-8114-417a-a20b-796df5612ac9"/>
@@ -1699,12 +2538,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19232968-D0AD-4578-90F9-FB7793DCA679}">
   <ds:schemaRefs>
@@ -1714,6 +2547,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99010E58-C46F-4EC0-AEBC-FB07528535B3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="5b1997fb-8114-417a-a20b-796df5612ac9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="eefc82e4-fec2-46ce-83e1-5271053f7c9b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{24CD1E4A-6B0F-4C5B-8CAD-007A87F29157}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1730,21 +2580,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{99010E58-C46F-4EC0-AEBC-FB07528535B3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="5b1997fb-8114-417a-a20b-796df5612ac9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="eefc82e4-fec2-46ce-83e1-5271053f7c9b"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>